<commit_message>
Update List of Eligible Participants_revised 240401.xlsx
</commit_message>
<xml_diff>
--- a/frontend/public/external/List of Eligible Participants_revised 240401.xlsx
+++ b/frontend/public/external/List of Eligible Participants_revised 240401.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moses Lee\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moses Lee\Desktop\Github\ecss-cms\frontend\public\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300918CD-4C50-4F19-822B-C503EAE4BCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DEB146-6243-44FA-B423-4FFF2624A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,13 +365,13 @@
     <t>Rosalind Ong</t>
   </si>
   <si>
-    <t>Deputy Head, Operations</t>
-  </si>
-  <si>
     <t>En Community Services Society</t>
   </si>
   <si>
     <t>Receipt No / SF Invoice No</t>
+  </si>
+  <si>
+    <t>Programme Manager</t>
   </si>
 </sst>
 </file>
@@ -1111,6 +1111,108 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1122,6 +1224,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1139,111 +1244,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1791,7 +1791,7 @@
   <dimension ref="A1:V159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD72"/>
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1860,13 +1860,13 @@
       <c r="A4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="B4" s="113" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -1886,29 +1886,29 @@
       <c r="A5" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
       <c r="E5" s="54"/>
       <c r="F5" s="54"/>
       <c r="G5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="114" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="83"/>
+      <c r="I5" s="114"/>
       <c r="J5" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="83" t="s">
+      <c r="K5" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="7"/>
@@ -1939,32 +1939,32 @@
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:22" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="86" t="s">
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="86"/>
-      <c r="Q7" s="86"/>
-      <c r="R7" s="88" t="s">
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="89"/>
-      <c r="T7" s="90"/>
+      <c r="S7" s="121"/>
+      <c r="T7" s="122"/>
       <c r="U7" s="13" t="s">
         <v>30</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>25</v>
       </c>
       <c r="V8" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="33" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -5293,26 +5293,26 @@
       <c r="E146" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F146" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="G146" s="82"/>
-      <c r="H146" s="82"/>
-      <c r="I146" s="82"/>
-      <c r="J146" s="82"/>
+      <c r="F146" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="G146" s="113"/>
+      <c r="H146" s="113"/>
+      <c r="I146" s="113"/>
+      <c r="J146" s="113"/>
       <c r="K146" s="9"/>
-      <c r="L146" s="84" t="s">
+      <c r="L146" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="M146" s="106"/>
-      <c r="N146" s="106"/>
-      <c r="O146" s="106"/>
-      <c r="P146" s="106"/>
-      <c r="Q146" s="106"/>
-      <c r="R146" s="106"/>
-      <c r="S146" s="106"/>
-      <c r="T146" s="106"/>
-      <c r="U146" s="85"/>
+      <c r="M146" s="116"/>
+      <c r="N146" s="116"/>
+      <c r="O146" s="116"/>
+      <c r="P146" s="116"/>
+      <c r="Q146" s="116"/>
+      <c r="R146" s="116"/>
+      <c r="S146" s="116"/>
+      <c r="T146" s="116"/>
+      <c r="U146" s="117"/>
     </row>
     <row r="147" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="22" t="s">
@@ -5328,21 +5328,21 @@
       <c r="I147" s="37"/>
       <c r="J147" s="9"/>
       <c r="K147" s="9"/>
-      <c r="L147" s="91" t="s">
+      <c r="L147" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="M147" s="121"/>
-      <c r="N147" s="121"/>
-      <c r="O147" s="121"/>
-      <c r="P147" s="121"/>
-      <c r="Q147" s="121"/>
-      <c r="R147" s="121"/>
-      <c r="S147" s="121"/>
-      <c r="T147" s="121"/>
-      <c r="U147" s="92"/>
+      <c r="M147" s="84"/>
+      <c r="N147" s="84"/>
+      <c r="O147" s="84"/>
+      <c r="P147" s="84"/>
+      <c r="Q147" s="84"/>
+      <c r="R147" s="84"/>
+      <c r="S147" s="84"/>
+      <c r="T147" s="84"/>
+      <c r="U147" s="85"/>
     </row>
     <row r="148" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="122"/>
+      <c r="A148" s="82"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
       <c r="D148" s="37"/>
@@ -5353,33 +5353,33 @@
       <c r="I148" s="37"/>
       <c r="J148" s="9"/>
       <c r="K148" s="9"/>
-      <c r="L148" s="93" t="s">
+      <c r="L148" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="M148" s="120"/>
-      <c r="N148" s="120"/>
-      <c r="O148" s="120"/>
-      <c r="P148" s="120"/>
-      <c r="Q148" s="120"/>
-      <c r="R148" s="120"/>
-      <c r="S148" s="120"/>
-      <c r="T148" s="120"/>
-      <c r="U148" s="94"/>
+      <c r="M148" s="87"/>
+      <c r="N148" s="87"/>
+      <c r="O148" s="87"/>
+      <c r="P148" s="87"/>
+      <c r="Q148" s="87"/>
+      <c r="R148" s="87"/>
+      <c r="S148" s="87"/>
+      <c r="T148" s="87"/>
+      <c r="U148" s="88"/>
     </row>
     <row r="149" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A149" s="96" t="s">
+      <c r="A149" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="B149" s="119"/>
-      <c r="C149" s="119"/>
-      <c r="D149" s="119"/>
-      <c r="E149" s="119"/>
-      <c r="F149" s="119"/>
-      <c r="G149" s="119"/>
-      <c r="H149" s="119"/>
-      <c r="I149" s="119"/>
-      <c r="J149" s="119"/>
-      <c r="K149" s="97"/>
+      <c r="B149" s="91"/>
+      <c r="C149" s="91"/>
+      <c r="D149" s="91"/>
+      <c r="E149" s="91"/>
+      <c r="F149" s="91"/>
+      <c r="G149" s="91"/>
+      <c r="H149" s="91"/>
+      <c r="I149" s="91"/>
+      <c r="J149" s="91"/>
+      <c r="K149" s="92"/>
       <c r="L149" s="28"/>
       <c r="M149" s="58"/>
       <c r="N149" s="58"/>
@@ -5392,19 +5392,19 @@
       <c r="U149" s="59"/>
     </row>
     <row r="150" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="98" t="s">
+      <c r="A150" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="B150" s="118"/>
-      <c r="C150" s="118"/>
-      <c r="D150" s="118"/>
-      <c r="E150" s="118"/>
-      <c r="F150" s="118"/>
-      <c r="G150" s="118"/>
-      <c r="H150" s="118"/>
-      <c r="I150" s="118"/>
-      <c r="J150" s="118"/>
-      <c r="K150" s="99"/>
+      <c r="B150" s="94"/>
+      <c r="C150" s="94"/>
+      <c r="D150" s="94"/>
+      <c r="E150" s="94"/>
+      <c r="F150" s="94"/>
+      <c r="G150" s="94"/>
+      <c r="H150" s="94"/>
+      <c r="I150" s="94"/>
+      <c r="J150" s="94"/>
+      <c r="K150" s="95"/>
       <c r="L150" s="28"/>
       <c r="M150" s="58"/>
       <c r="N150" s="58"/>
@@ -5417,17 +5417,17 @@
       <c r="U150" s="59"/>
     </row>
     <row r="151" spans="1:21" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="98"/>
-      <c r="B151" s="118"/>
-      <c r="C151" s="118"/>
-      <c r="D151" s="118"/>
-      <c r="E151" s="118"/>
-      <c r="F151" s="118"/>
-      <c r="G151" s="118"/>
-      <c r="H151" s="118"/>
-      <c r="I151" s="118"/>
-      <c r="J151" s="118"/>
-      <c r="K151" s="99"/>
+      <c r="A151" s="93"/>
+      <c r="B151" s="94"/>
+      <c r="C151" s="94"/>
+      <c r="D151" s="94"/>
+      <c r="E151" s="94"/>
+      <c r="F151" s="94"/>
+      <c r="G151" s="94"/>
+      <c r="H151" s="94"/>
+      <c r="I151" s="94"/>
+      <c r="J151" s="94"/>
+      <c r="K151" s="95"/>
       <c r="L151" s="28"/>
       <c r="M151" s="58"/>
       <c r="N151" s="58"/>
@@ -5440,19 +5440,19 @@
       <c r="U151" s="59"/>
     </row>
     <row r="152" spans="1:21" ht="43.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="100" t="s">
+      <c r="A152" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B152" s="117"/>
-      <c r="C152" s="117"/>
-      <c r="D152" s="117"/>
-      <c r="E152" s="117"/>
-      <c r="F152" s="117"/>
-      <c r="G152" s="117"/>
-      <c r="H152" s="117"/>
-      <c r="I152" s="117"/>
-      <c r="J152" s="117"/>
-      <c r="K152" s="101"/>
+      <c r="B152" s="97"/>
+      <c r="C152" s="97"/>
+      <c r="D152" s="97"/>
+      <c r="E152" s="97"/>
+      <c r="F152" s="97"/>
+      <c r="G152" s="97"/>
+      <c r="H152" s="97"/>
+      <c r="I152" s="97"/>
+      <c r="J152" s="97"/>
+      <c r="K152" s="98"/>
       <c r="L152" s="61"/>
       <c r="M152" s="9"/>
       <c r="N152" s="9"/>
@@ -5465,17 +5465,17 @@
       <c r="U152" s="59"/>
     </row>
     <row r="153" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="102"/>
-      <c r="B153" s="116"/>
-      <c r="C153" s="116"/>
-      <c r="D153" s="116"/>
-      <c r="E153" s="116"/>
-      <c r="F153" s="116"/>
-      <c r="G153" s="116"/>
-      <c r="H153" s="116"/>
-      <c r="I153" s="116"/>
-      <c r="J153" s="116"/>
-      <c r="K153" s="103"/>
+      <c r="A153" s="99"/>
+      <c r="B153" s="100"/>
+      <c r="C153" s="100"/>
+      <c r="D153" s="100"/>
+      <c r="E153" s="100"/>
+      <c r="F153" s="100"/>
+      <c r="G153" s="100"/>
+      <c r="H153" s="100"/>
+      <c r="I153" s="100"/>
+      <c r="J153" s="100"/>
+      <c r="K153" s="101"/>
       <c r="L153" s="61"/>
       <c r="M153" s="9"/>
       <c r="N153" s="9"/>
@@ -5488,9 +5488,9 @@
       <c r="U153" s="59"/>
     </row>
     <row r="154" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="107"/>
-      <c r="B154" s="108"/>
-      <c r="C154" s="109"/>
+      <c r="A154" s="102"/>
+      <c r="B154" s="103"/>
+      <c r="C154" s="104"/>
       <c r="D154" s="62"/>
       <c r="E154" s="38"/>
       <c r="F154" s="38"/>
@@ -5511,9 +5511,9 @@
       <c r="U154" s="59"/>
     </row>
     <row r="155" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="110"/>
-      <c r="B155" s="111"/>
-      <c r="C155" s="112"/>
+      <c r="A155" s="105"/>
+      <c r="B155" s="106"/>
+      <c r="C155" s="107"/>
       <c r="D155" s="62"/>
       <c r="E155" s="39"/>
       <c r="F155" s="39"/>
@@ -5534,9 +5534,9 @@
       <c r="U155" s="59"/>
     </row>
     <row r="156" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="113"/>
-      <c r="B156" s="114"/>
-      <c r="C156" s="115"/>
+      <c r="A156" s="108"/>
+      <c r="B156" s="109"/>
+      <c r="C156" s="110"/>
       <c r="D156" s="62"/>
       <c r="E156" s="9"/>
       <c r="F156" s="9"/>
@@ -5557,11 +5557,11 @@
       <c r="U156" s="59"/>
     </row>
     <row r="157" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A157" s="104" t="s">
+      <c r="A157" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="B157" s="105"/>
-      <c r="C157" s="105"/>
+      <c r="B157" s="112"/>
+      <c r="C157" s="112"/>
       <c r="D157" s="63"/>
       <c r="E157" s="24"/>
       <c r="F157" s="24"/>
@@ -5582,14 +5582,23 @@
       <c r="U157" s="60"/>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="95" t="s">
+      <c r="A159" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="B159" s="95"/>
+      <c r="B159" s="89"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="18">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="L146:U146"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="F146:J146"/>
+    <mergeCell ref="R7:T7"/>
     <mergeCell ref="L147:U147"/>
     <mergeCell ref="L148:U148"/>
     <mergeCell ref="A159:B159"/>
@@ -5599,15 +5608,6 @@
     <mergeCell ref="A153:K153"/>
     <mergeCell ref="A154:C156"/>
     <mergeCell ref="A157:C157"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="L146:U146"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="F146:J146"/>
-    <mergeCell ref="R7:T7"/>
   </mergeCells>
   <conditionalFormatting sqref="B146:B147">
     <cfRule type="containsBlanks" dxfId="5" priority="1">

</xml_diff>